<commit_message>
fix error and update file test.xls
</commit_message>
<xml_diff>
--- a/03. Documents/Test20180629.xlsx
+++ b/03. Documents/Test20180629.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project QuanLyKhachHang" sheetId="1" r:id="rId1"/>
+    <sheet name="Error" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>stt</t>
   </si>
@@ -57,13 +58,52 @@
   </si>
   <si>
     <t>Thành</t>
+  </si>
+  <si>
+    <t>Không bắt được exception kết nối lỗi tới database khi đăng nhập</t>
+  </si>
+  <si>
+    <t>Chuyển thành bắt sqlexception</t>
+  </si>
+  <si>
+    <t>Trong sự kiện click button login chưa bắt sqlexception</t>
+  </si>
+  <si>
+    <t>Tham khảo</t>
+  </si>
+  <si>
+    <t>Error 1</t>
+  </si>
+  <si>
+    <t>Mất cạnh của table</t>
+  </si>
+  <si>
+    <t>Thêm border bo ngoài table</t>
+  </si>
+  <si>
+    <t>Error 2</t>
+  </si>
+  <si>
+    <t>Không nhập được dấu " - " hoặc dấu cách trong ô textbox điền số điện thoại</t>
+  </si>
+  <si>
+    <t>Do lỗi bắt điều kiện khi nhập không cho điền dấu cách hoặc kí tự cần điền</t>
+  </si>
+  <si>
+    <t>Do độ rộng màn hình khác nhau trên mỗi máy tính</t>
+  </si>
+  <si>
+    <t>Error 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm điều kiện cho nhập dấu </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,15 +119,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +145,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -139,11 +199,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,17 +213,34 @@
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -177,6 +255,315 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="419100"/>
+          <a:ext cx="5467350" cy="6238875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="466725" y="5876925"/>
+          <a:ext cx="3686175" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57471</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5543871" y="390525"/>
+          <a:ext cx="10924854" cy="6257926"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>207924</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>56236</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6838950"/>
+          <a:ext cx="13009524" cy="7314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>207924</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>75286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="15811500"/>
+          <a:ext cx="13009524" cy="7314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>141409</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>114071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="24193500"/>
+          <a:ext cx="11723809" cy="1828571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>207924</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>75286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="26289000"/>
+          <a:ext cx="13009524" cy="7314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,93 +829,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -536,9 +967,10 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -546,9 +978,10 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -556,9 +989,10 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -566,9 +1000,10 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -576,9 +1011,10 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -586,9 +1022,10 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -596,9 +1033,10 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -606,9 +1044,10 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -616,10 +1055,485 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" location="Error!A2" display="Error 1"/>
+    <hyperlink ref="G4" location="Error!A82" display="Error 2"/>
+    <hyperlink ref="G5" location="Error!A126" display="Error 3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J126"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B126" s="12"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+      <c r="G126" s="12"/>
+      <c r="H126" s="12"/>
+      <c r="I126" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A126:I126"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edit file test for Thanh
</commit_message>
<xml_diff>
--- a/03. Documents/Test20180629.xlsx
+++ b/03. Documents/Test20180629.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockProjects\QuanLyKhachHang\03. Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="Project QuanLyKhachHang" sheetId="1" r:id="rId1"/>
     <sheet name="Error" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +24,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tung</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sau khi sửa được một lỗi, ghi log comment vào để theo dõi cách xử lý.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mỗi một lỗi nên để một sheet để tiện theo dõi hơn</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>stt</t>
   </si>
@@ -97,13 +155,16 @@
   </si>
   <si>
     <t xml:space="preserve">Thêm điều kiện cho nhập dấu </t>
+  </si>
+  <si>
+    <t>Log Comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +194,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -828,11 +902,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,12 +915,12 @@
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="38.140625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="5" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -863,13 +937,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -885,12 +962,13 @@
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -906,14 +984,15 @@
       <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -929,14 +1008,15 @@
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -952,14 +1032,15 @@
       <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -967,10 +1048,11 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -978,10 +1060,11 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -989,10 +1072,11 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1000,10 +1084,11 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1011,10 +1096,11 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1022,10 +1108,11 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1033,10 +1120,11 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1044,10 +1132,11 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1055,17 +1144,19 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" location="Error!A2" display="Error 1"/>
-    <hyperlink ref="G4" location="Error!A82" display="Error 2"/>
-    <hyperlink ref="G5" location="Error!A126" display="Error 3"/>
+    <hyperlink ref="H3" location="Error!A2" display="Error 1"/>
+    <hyperlink ref="H4" location="Error!A82" display="Error 2"/>
+    <hyperlink ref="H5" location="Error!A126" display="Error 3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1073,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>

</xml_diff>